<commit_message>
Added step files of the off-the-shelf components
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Planform" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="PER3_8x38SF" sheetId="14" r:id="rId12"/>
     <sheet name="MassBalance" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="145621" iterateCount="1000" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2217" uniqueCount="1642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2221" uniqueCount="1646">
   <si>
     <t>Scale size</t>
   </si>
@@ -4957,16 +4957,29 @@
   </si>
   <si>
     <t xml:space="preserve">        90.8        0.80     -0.0566     -0.0010      0.0136       0.121       0.510      -0.028              </t>
+  </si>
+  <si>
+    <t>Root interpolated</t>
+  </si>
+  <si>
+    <t>Arduino Uno and shield: 60gr</t>
+  </si>
+  <si>
+    <t>Receiver small: 4gr</t>
+  </si>
+  <si>
+    <t>Receiver large: 8gr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -5055,7 +5068,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5074,6 +5087,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5250,7 +5265,7 @@
             <c:numRef>
               <c:f>Airfoil!$AW$8:$AW$126</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="119"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -5616,7 +5631,7 @@
             <c:numRef>
               <c:f>Airfoil!$AX$8:$AX$126</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="119"/>
                 <c:pt idx="0">
                   <c:v>6.9999999999999999E-4</c:v>
@@ -6052,7 +6067,7 @@
             <c:numRef>
               <c:f>Airfoil!$K$8:$K$86</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>0.99839</c:v>
@@ -6298,7 +6313,7 @@
             <c:numRef>
               <c:f>Airfoil!$L$8:$L$86</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>1.5949999999999999E-2</c:v>
@@ -6555,11 +6570,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="480749440"/>
-        <c:axId val="480750976"/>
+        <c:axId val="120317440"/>
+        <c:axId val="120318976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="480749440"/>
+        <c:axId val="120317440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6597,12 +6612,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480750976"/>
+        <c:crossAx val="120318976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="480750976"/>
+        <c:axId val="120318976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6650,7 +6665,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480749440"/>
+        <c:crossAx val="120317440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6983,11 +6998,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="483819904"/>
-        <c:axId val="483821440"/>
+        <c:axId val="151896448"/>
+        <c:axId val="151897984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="483819904"/>
+        <c:axId val="151896448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7025,12 +7040,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483821440"/>
+        <c:crossAx val="151897984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="483821440"/>
+        <c:axId val="151897984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7078,7 +7093,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483819904"/>
+        <c:crossAx val="151896448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7373,11 +7388,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="483830400"/>
-        <c:axId val="483836288"/>
+        <c:axId val="151980672"/>
+        <c:axId val="151982464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="483830400"/>
+        <c:axId val="151980672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7415,12 +7430,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483836288"/>
+        <c:crossAx val="151982464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="483836288"/>
+        <c:axId val="151982464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7468,7 +7483,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483830400"/>
+        <c:crossAx val="151980672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8170,7 +8185,7 @@
             <c:numRef>
               <c:f>Airfoil!$K$8:$K$86</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>0.99839</c:v>
@@ -8416,7 +8431,7 @@
             <c:numRef>
               <c:f>Airfoil!$L$8:$L$86</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>1.5949999999999999E-2</c:v>
@@ -8673,11 +8688,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="483862016"/>
-        <c:axId val="483863552"/>
+        <c:axId val="151991808"/>
+        <c:axId val="151993344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="483862016"/>
+        <c:axId val="151991808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8715,12 +8730,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483863552"/>
+        <c:crossAx val="151993344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="483863552"/>
+        <c:axId val="151993344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8768,7 +8783,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483862016"/>
+        <c:crossAx val="151991808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8835,6 +8850,1557 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.3514412872303999E-2"/>
+          <c:y val="4.7214074282423218E-2"/>
+          <c:w val="0.87474946935980824"/>
+          <c:h val="0.90557185143515351"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Airfoil!$N$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Root interpolated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="BE4B48"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="BE4B48"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Airfoil!$M$8:$M$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="119"/>
+                <c:pt idx="0">
+                  <c:v>0.99839</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99331000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98663999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97729299999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96564300000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95215000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.93696299999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.91901699999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.89695999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.87058899999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.82386999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.80437999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.72114</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.69133999999999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.66071999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.62941000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.59755000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.56525999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.53269999999999995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.46729999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.43474000000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.40244999999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.37058999999999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.33928000000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.30865999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.27886</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.22220999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.19561999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.17033000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.14645</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.13136200000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.12408</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.116976</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.110054</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.10332</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.6777000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.0426000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.4269999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.8311000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7.2548000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.6989999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.1636999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.6492000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.1560000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.6843999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.8059999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.0148999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.6530000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.3139E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.9975E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.704E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.4333E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.1854999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9.6100000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7.5989999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.8219999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.28E-3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.9729999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.903E-3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.07E-3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.75E-4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.1900000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.1900000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.75E-4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.07E-3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.903E-3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.9729999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.28E-3</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.8219999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.5989999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>9.6100000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.1854999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.4333E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.704E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.9975E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.3139E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2.6530000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.0148999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.3994999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.8059999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.2342999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.1560000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6.1636999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6.6989999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>7.2548000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.4269999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.10332</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.12408</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.14645</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.17033000000000001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.19561999999999999</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.22220999999999999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.27886</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.30865999999999999</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.40244999999999997</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.46729999999999999</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.53269999999999995</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.59755000000000003</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.62941000000000003</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.66071999999999997</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.69133999999999995</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.72114</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.77778999999999998</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.80437999999999998</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.81008000000000002</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.82004999999999995</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.84077800000000003</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.86804099999999995</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.89553000000000005</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.91827400000000003</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.95184000000000002</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.98662000000000005</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.99839</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Airfoil!$N$8:$N$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="119"/>
+                <c:pt idx="0">
+                  <c:v>1.5949999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5744000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5800000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5980999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6378E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8301999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0324999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3550000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.809E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.6900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0730000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.6680000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.2179999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.7680000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.3120000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.8399999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.3409999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.7999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.2009999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.5299999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.7769999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.9360000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.9709999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.8460000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.6320000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.3390000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.9779999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.5529999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.072E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.5389999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.1596000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.9629999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.7615999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.5555000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.3450000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.1303000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.9119999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.6910000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.4678999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.2430999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.0169999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.7892999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.5573000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.3180000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.07E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.5749999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.1178000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.8969999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.6741999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.444E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.2009999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.9428000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.6794E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.4239999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.1877E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9.7389999999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7.8399999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6.1869999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.7590000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.5300000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.4429999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.3320000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-1.67E-3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-3.4919999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-5.1999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-6.5970000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-7.757E-3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-8.8199999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-9.8989999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-1.0987E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-1.205E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-1.3063E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-1.4043999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-1.502E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-1.6012999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-1.7011999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-1.8956000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-1.9843E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-2.0619999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-2.1264999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-2.2370000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-2.3522999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-2.4060000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-2.4521000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-2.5239999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-2.598E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-2.6419999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-2.6530000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-2.631E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-2.5839999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-2.512E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-2.419E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-2.308E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-2.1839999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-1.754E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-1.451E-2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-1.3010000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-1.1560000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-8.8500000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-7.6099999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-6.4599999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-5.4200000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-4.4799999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-3.64E-3</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-2.9099999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-2.2699999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-2.3319999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-1.9400000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>-9.2800000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>6.2200000000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>2.5500000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>4.6979999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>9.0799999999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.4109999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.5949999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-920B-4C24-950F-2494D9334278}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Airfoil!$K$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Airfoil Section Centreline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="4A7EBB"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4A7EBB"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Airfoil!$K$8:$K$86</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="79"/>
+                <c:pt idx="0">
+                  <c:v>0.99839</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98663999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95215000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89695999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82386999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80437999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.77778999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.72114</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.69133999999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.66071999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.62941000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.59755000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56525999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.53269999999999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.46729999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.43474000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.40244999999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.37058999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.33928000000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.30865999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.27886</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.22220999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.19561999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.17033000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.14645</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.12408</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.10332</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.4269999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.6989999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.1560000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.8059999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.6530000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.704E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.6100000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.28E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.07E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.07E-3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.28E-3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.6100000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.704E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.6530000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.8059999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.1560000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.6989999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8.4269999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.10332</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.12408</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.14645</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.17033000000000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.19561999999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.22220999999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.27886</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.30865999999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.33928000000000003</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.37058999999999997</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.40244999999999997</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.43474000000000002</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.46729999999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.53269999999999995</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.56525999999999998</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.59755000000000003</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.62941000000000003</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.66071999999999997</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.69133999999999995</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.72114</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.77778999999999998</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.80437999999999998</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.82004999999999995</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.89553000000000005</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.95184000000000002</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.98662000000000005</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.99839</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Airfoil!$L$8:$L$86</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="79"/>
+                <c:pt idx="0">
+                  <c:v>1.5949999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5800000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3550000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0730000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.5900000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1240000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.6680000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.2179999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.7680000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.3120000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.8399999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.3409999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.7999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.2009999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.5299999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.7769999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.9360000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.9709999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.8460000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.6320000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.3390000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.9779999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.5529999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.072E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.5389999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.9629999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.3450000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.6910000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.0169999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.3180000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.5749999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.8969999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.2009999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.4239999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.8399999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.5300000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-5.1999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-8.8199999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-1.205E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.502E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-2.0619999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-2.2370000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-2.4060000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-2.5239999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-2.598E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-2.6419999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-2.6530000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-2.631E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-2.5839999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-2.512E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-2.419E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-2.308E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-2.1839999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-2.0469999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-1.9040000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-1.754E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-1.602E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-1.451E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-1.3010000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-1.1560000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-1.017E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-8.8500000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-7.6099999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-6.4599999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-5.4200000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-4.4799999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-3.64E-3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-2.9099999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-2.2699999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-1.9400000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.5500000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>9.0799999999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.4109999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.5949999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-920B-4C24-950F-2494D9334278}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="152581248"/>
+        <c:axId val="152582784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="152581248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="152582784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="152582784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="878787"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="152581248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -8967,11 +10533,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="508175872"/>
-        <c:axId val="508177408"/>
+        <c:axId val="154690688"/>
+        <c:axId val="154692224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="508175872"/>
+        <c:axId val="154690688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8981,12 +10547,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="508177408"/>
+        <c:crossAx val="154692224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="508177408"/>
+        <c:axId val="154692224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8997,13 +10563,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="508175872"/>
+        <c:crossAx val="154690688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9521,6 +11088,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>128940</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -17471,8 +19076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O457"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="M144" sqref="M144"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="I124" sqref="I124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23569,13 +25174,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:C8"/>
+  <dimension ref="A6:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -23596,6 +25204,30 @@
       </c>
       <c r="C8">
         <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1643</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1644</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -23608,19 +25240,31 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:BD126"/>
   <sheetViews>
-    <sheetView topLeftCell="AR1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AT29" sqref="AT29"/>
+    <sheetView topLeftCell="K1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="11" width="8.5703125"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="49" width="8.5703125"/>
+    <col min="50" max="50" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
+      <c r="K2">
+        <f>COUNT(K8:K86)</f>
+        <v>79</v>
+      </c>
+      <c r="AW2">
+        <f>COUNT(AW8:AW126)</f>
+        <v>119</v>
+      </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -23689,8 +25333,8 @@
       <c r="M6" t="s">
         <v>30</v>
       </c>
-      <c r="N6">
-        <v>2</v>
+      <c r="N6" t="s">
+        <v>1642</v>
       </c>
       <c r="O6" t="s">
         <v>30</v>
@@ -23950,16 +25594,22 @@
         <f t="shared" si="0"/>
         <v>0.15538666330505518</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="18">
         <v>0.99839</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="18">
         <v>1.5949999999999999E-2</v>
       </c>
-      <c r="AW8">
+      <c r="M8">
+        <v>0.99839</v>
+      </c>
+      <c r="N8">
+        <v>1.5949999999999999E-2</v>
+      </c>
+      <c r="AW8" s="18">
         <v>1</v>
       </c>
-      <c r="AX8">
+      <c r="AX8" s="18">
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="AZ8">
@@ -23988,16 +25638,22 @@
         <f t="shared" si="0"/>
         <v>0.15530637815946341</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="18">
         <v>0.98663999999999996</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="18">
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="AW9">
+      <c r="M9">
+        <v>0.99331000000000003</v>
+      </c>
+      <c r="N9">
+        <v>1.5744000000000001E-2</v>
+      </c>
+      <c r="AW9" s="18">
         <v>0.96091000000000004</v>
       </c>
-      <c r="AX9">
+      <c r="AX9" s="18">
         <v>4.28E-3</v>
       </c>
       <c r="AZ9">
@@ -24026,16 +25682,22 @@
         <f t="shared" si="0"/>
         <v>0.15403752379326352</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="18">
         <v>0.95215000000000005</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="18">
         <v>1.7100000000000001E-2</v>
       </c>
-      <c r="AW10">
+      <c r="M10">
+        <v>0.98663999999999996</v>
+      </c>
+      <c r="N10">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="AW10" s="18">
         <v>0.94833000000000001</v>
       </c>
-      <c r="AX10">
+      <c r="AX10" s="18">
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="AZ10">
@@ -24064,16 +25726,22 @@
         <f t="shared" si="0"/>
         <v>0.15149632440235977</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="18">
         <v>0.89695999999999998</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="18">
         <v>2.3550000000000001E-2</v>
       </c>
-      <c r="AW11">
+      <c r="M11">
+        <v>0.97729299999999997</v>
+      </c>
+      <c r="N11">
+        <v>1.5980999999999999E-2</v>
+      </c>
+      <c r="AW11" s="18">
         <v>0.93571000000000004</v>
       </c>
-      <c r="AX11">
+      <c r="AX11" s="18">
         <v>6.5399999999999998E-3</v>
       </c>
       <c r="AZ11">
@@ -24102,16 +25770,22 @@
         <f t="shared" si="0"/>
         <v>0.14759376819490047</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="18">
         <v>0.82386999999999999</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="18">
         <v>3.6900000000000002E-2</v>
       </c>
-      <c r="AW12">
+      <c r="M12">
+        <v>0.96564300000000003</v>
+      </c>
+      <c r="N12">
+        <v>1.6378E-2</v>
+      </c>
+      <c r="AW12" s="18">
         <v>0.92306999999999995</v>
       </c>
-      <c r="AX12">
+      <c r="AX12" s="18">
         <v>7.6899999999999998E-3</v>
       </c>
       <c r="AZ12">
@@ -24140,16 +25814,22 @@
         <f t="shared" si="0"/>
         <v>0.1422303714035219</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="18">
         <v>0.80437999999999998</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="18">
         <v>4.0730000000000002E-2</v>
       </c>
-      <c r="AW13">
+      <c r="M13">
+        <v>0.95215000000000005</v>
+      </c>
+      <c r="N13">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="AW13" s="18">
         <v>0.89778000000000002</v>
       </c>
-      <c r="AX13">
+      <c r="AX13" s="18">
         <v>9.9900000000000006E-3</v>
       </c>
       <c r="AZ13">
@@ -24178,16 +25858,22 @@
         <f t="shared" si="0"/>
         <v>0.13530141427310441</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="18">
         <v>0.77778999999999998</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="18">
         <v>4.5900000000000003E-2</v>
       </c>
-      <c r="AW14">
+      <c r="M14">
+        <v>0.93696299999999999</v>
+      </c>
+      <c r="N14">
+        <v>1.8301999999999999E-2</v>
+      </c>
+      <c r="AW14" s="18">
         <v>0.88514999999999999</v>
       </c>
-      <c r="AX14">
+      <c r="AX14" s="18">
         <v>1.1140000000000001E-2</v>
       </c>
       <c r="AZ14">
@@ -24216,16 +25902,22 @@
         <f t="shared" si="0"/>
         <v>0.12669694106077237</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="18">
         <v>0.75</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="18">
         <v>5.1240000000000001E-2</v>
       </c>
-      <c r="AW15">
+      <c r="M15">
+        <v>0.91901699999999997</v>
+      </c>
+      <c r="N15">
+        <v>2.0324999999999999E-2</v>
+      </c>
+      <c r="AW15" s="18">
         <v>0.84728000000000003</v>
       </c>
-      <c r="AX15">
+      <c r="AX15" s="18">
         <v>1.455E-2</v>
       </c>
       <c r="AZ15">
@@ -24254,16 +25946,22 @@
         <f t="shared" si="0"/>
         <v>0.11629826937739017</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="18">
         <v>0.72114</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="18">
         <v>5.6680000000000001E-2</v>
       </c>
-      <c r="AW16">
+      <c r="M16">
+        <v>0.89695999999999998</v>
+      </c>
+      <c r="N16">
+        <v>2.3550000000000001E-2</v>
+      </c>
+      <c r="AW16" s="18">
         <v>0.82206000000000001</v>
       </c>
-      <c r="AX16">
+      <c r="AX16" s="18">
         <v>1.6789999999999999E-2</v>
       </c>
       <c r="AZ16">
@@ -24292,16 +25990,22 @@
         <f t="shared" si="0"/>
         <v>0.10398497150457017</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="18">
         <v>0.69133999999999995</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="18">
         <v>6.2179999999999999E-2</v>
       </c>
-      <c r="AW17">
+      <c r="M17">
+        <v>0.87058899999999995</v>
+      </c>
+      <c r="N17">
+        <v>2.809E-2</v>
+      </c>
+      <c r="AW17" s="18">
         <v>0.80944000000000005</v>
       </c>
-      <c r="AX17">
+      <c r="AX17" s="18">
         <v>1.789E-2</v>
       </c>
       <c r="AZ17">
@@ -24330,16 +26034,22 @@
         <f t="shared" si="0"/>
         <v>8.9643601040932747E-2</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="18">
         <v>0.66071999999999997</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="18">
         <v>6.7680000000000004E-2</v>
       </c>
-      <c r="AW18">
+      <c r="M18">
+        <v>0.82386999999999999</v>
+      </c>
+      <c r="N18">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="AW18" s="18">
         <v>0.79683000000000004</v>
       </c>
-      <c r="AX18">
+      <c r="AX18" s="18">
         <v>1.898E-2</v>
       </c>
       <c r="AZ18">
@@ -24368,16 +26078,22 @@
         <f t="shared" si="0"/>
         <v>7.3176419548366262E-2</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="18">
         <v>0.62941000000000003</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="18">
         <v>7.3120000000000004E-2</v>
       </c>
-      <c r="AW19">
+      <c r="M19">
+        <v>0.80437999999999998</v>
+      </c>
+      <c r="N19">
+        <v>4.0730000000000002E-2</v>
+      </c>
+      <c r="AW19" s="18">
         <v>0.78422000000000003</v>
       </c>
-      <c r="AX19">
+      <c r="AX19" s="18">
         <v>2.0060000000000001E-2</v>
       </c>
       <c r="AZ19">
@@ -24406,16 +26122,22 @@
         <f t="shared" si="0"/>
         <v>5.4546775112578778E-2</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="18">
         <v>0.59755000000000003</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="18">
         <v>7.8399999999999997E-2</v>
       </c>
-      <c r="AW20">
+      <c r="M20">
+        <v>0.72114</v>
+      </c>
+      <c r="N20">
+        <v>5.6680000000000001E-2</v>
+      </c>
+      <c r="AW20" s="18">
         <v>0.77159999999999995</v>
       </c>
-      <c r="AX20">
+      <c r="AX20" s="18">
         <v>2.1129999999999999E-2</v>
       </c>
       <c r="AZ20">
@@ -24444,16 +26166,22 @@
         <f t="shared" si="0"/>
         <v>3.3848915513178028E-2</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="18">
         <v>0.56525999999999998</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="18">
         <v>8.3409999999999998E-2</v>
       </c>
-      <c r="AW21">
+      <c r="M21">
+        <v>0.69133999999999995</v>
+      </c>
+      <c r="N21">
+        <v>6.2179999999999999E-2</v>
+      </c>
+      <c r="AW21" s="18">
         <v>0.73373999999999995</v>
       </c>
-      <c r="AX21">
+      <c r="AX21" s="18">
         <v>2.4279999999999999E-2</v>
       </c>
       <c r="AZ21">
@@ -24482,16 +26210,22 @@
         <f t="shared" si="0"/>
         <v>1.1499974441390637E-2</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="18">
         <v>0.53269999999999995</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="18">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="AW22">
+      <c r="M22">
+        <v>0.66071999999999997</v>
+      </c>
+      <c r="N22">
+        <v>6.7680000000000004E-2</v>
+      </c>
+      <c r="AW22" s="18">
         <v>0.72111999999999998</v>
       </c>
-      <c r="AX22">
+      <c r="AX22" s="18">
         <v>2.5309999999999999E-2</v>
       </c>
       <c r="AZ22">
@@ -24520,16 +26254,22 @@
         <f t="shared" si="0"/>
         <v>-1.1199777810047613E-2</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="18">
         <v>0.5</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="18">
         <v>9.2009999999999995E-2</v>
       </c>
-      <c r="AW23">
+      <c r="M23">
+        <v>0.62941000000000003</v>
+      </c>
+      <c r="N23">
+        <v>7.3120000000000004E-2</v>
+      </c>
+      <c r="AW23" s="18">
         <v>0.69586999999999999</v>
       </c>
-      <c r="AX23">
+      <c r="AX23" s="18">
         <v>2.734E-2</v>
       </c>
       <c r="AZ23">
@@ -24558,16 +26298,22 @@
         <f t="shared" si="0"/>
         <v>-2.9192377068857158E-2</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="18">
         <v>0.46729999999999999</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="18">
         <v>9.5299999999999996E-2</v>
       </c>
-      <c r="AW24">
+      <c r="M24">
+        <v>0.59755000000000003</v>
+      </c>
+      <c r="N24">
+        <v>7.8399999999999997E-2</v>
+      </c>
+      <c r="AW24" s="18">
         <v>0.68325000000000002</v>
       </c>
-      <c r="AX24">
+      <c r="AX24" s="18">
         <v>2.8340000000000001E-2</v>
       </c>
       <c r="AZ24">
@@ -24586,16 +26332,22 @@
       </c>
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="K25">
+      <c r="K25" s="18">
         <v>0.43474000000000002</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="18">
         <v>9.7769999999999996E-2</v>
       </c>
-      <c r="AW25">
+      <c r="M25">
+        <v>0.56525999999999998</v>
+      </c>
+      <c r="N25">
+        <v>8.3409999999999998E-2</v>
+      </c>
+      <c r="AW25" s="18">
         <v>0.67062999999999995</v>
       </c>
-      <c r="AX25">
+      <c r="AX25" s="18">
         <v>2.9329999999999998E-2</v>
       </c>
       <c r="AZ25">
@@ -24614,16 +26366,22 @@
       </c>
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="K26">
+      <c r="K26" s="18">
         <v>0.40244999999999997</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="18">
         <v>9.9360000000000004E-2</v>
       </c>
-      <c r="AW26">
+      <c r="M26">
+        <v>0.53269999999999995</v>
+      </c>
+      <c r="N26">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="AW26" s="18">
         <v>0.65800999999999998</v>
       </c>
-      <c r="AX26">
+      <c r="AX26" s="18">
         <v>3.031E-2</v>
       </c>
       <c r="AZ26">
@@ -24642,16 +26400,22 @@
       </c>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="K27">
+      <c r="K27" s="18">
         <v>0.37058999999999997</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="18">
         <v>0.1</v>
       </c>
-      <c r="AW27">
+      <c r="M27">
+        <v>0.5</v>
+      </c>
+      <c r="N27">
+        <v>9.2009999999999995E-2</v>
+      </c>
+      <c r="AW27" s="18">
         <v>0.62017</v>
       </c>
-      <c r="AX27">
+      <c r="AX27" s="18">
         <v>3.3149999999999999E-2</v>
       </c>
       <c r="AZ27">
@@ -24670,16 +26434,22 @@
       </c>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="K28">
+      <c r="K28" s="18">
         <v>0.33928000000000003</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="18">
         <v>9.9709999999999993E-2</v>
       </c>
-      <c r="AW28">
+      <c r="M28">
+        <v>0.46729999999999999</v>
+      </c>
+      <c r="N28">
+        <v>9.5299999999999996E-2</v>
+      </c>
+      <c r="AW28" s="18">
         <v>0.60755999999999999</v>
       </c>
-      <c r="AX28">
+      <c r="AX28" s="18">
         <v>3.406E-2</v>
       </c>
       <c r="AZ28">
@@ -24698,16 +26468,22 @@
       </c>
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="K29">
+      <c r="K29" s="18">
         <v>0.30865999999999999</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="18">
         <v>9.8460000000000006E-2</v>
       </c>
-      <c r="AW29">
+      <c r="M29">
+        <v>0.43474000000000002</v>
+      </c>
+      <c r="N29">
+        <v>9.7769999999999996E-2</v>
+      </c>
+      <c r="AW29" s="18">
         <v>0.59494999999999998</v>
       </c>
-      <c r="AX29">
+      <c r="AX29" s="18">
         <v>3.4959999999999998E-2</v>
       </c>
       <c r="AZ29">
@@ -24726,16 +26502,22 @@
       </c>
     </row>
     <row r="30" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="K30">
+      <c r="K30" s="18">
         <v>0.27886</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="18">
         <v>9.6320000000000003E-2</v>
       </c>
-      <c r="AW30">
+      <c r="M30">
+        <v>0.40244999999999997</v>
+      </c>
+      <c r="N30">
+        <v>9.9360000000000004E-2</v>
+      </c>
+      <c r="AW30" s="18">
         <v>0.56974999999999998</v>
       </c>
-      <c r="AX30">
+      <c r="AX30" s="18">
         <v>3.6700000000000003E-2</v>
       </c>
       <c r="AZ30">
@@ -24748,16 +26530,22 @@
       </c>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="K31">
+      <c r="K31" s="18">
         <v>0.25</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="18">
         <v>9.3390000000000001E-2</v>
       </c>
-      <c r="AW31">
+      <c r="M31">
+        <v>0.37058999999999997</v>
+      </c>
+      <c r="N31">
+        <v>0.1</v>
+      </c>
+      <c r="AW31" s="18">
         <v>0.55715000000000003</v>
       </c>
-      <c r="AX31">
+      <c r="AX31" s="18">
         <v>3.7539999999999997E-2</v>
       </c>
       <c r="AZ31">
@@ -24770,16 +26558,22 @@
       </c>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="K32">
+      <c r="K32" s="18">
         <v>0.22220999999999999</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="18">
         <v>8.9779999999999999E-2</v>
       </c>
-      <c r="AW32">
+      <c r="M32">
+        <v>0.33928000000000003</v>
+      </c>
+      <c r="N32">
+        <v>9.9709999999999993E-2</v>
+      </c>
+      <c r="AW32" s="18">
         <v>0.54454999999999998</v>
       </c>
-      <c r="AX32">
+      <c r="AX32" s="18">
         <v>3.8359999999999998E-2</v>
       </c>
       <c r="AZ32">
@@ -24792,16 +26586,22 @@
       </c>
     </row>
     <row r="33" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K33">
+      <c r="K33" s="18">
         <v>0.19561999999999999</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="18">
         <v>8.5529999999999995E-2</v>
       </c>
-      <c r="AW33">
+      <c r="M33">
+        <v>0.30865999999999999</v>
+      </c>
+      <c r="N33">
+        <v>9.8460000000000006E-2</v>
+      </c>
+      <c r="AW33" s="18">
         <v>0.50678000000000001</v>
       </c>
-      <c r="AX33">
+      <c r="AX33" s="18">
         <v>4.0669999999999998E-2</v>
       </c>
       <c r="AZ33">
@@ -24814,16 +26614,22 @@
       </c>
     </row>
     <row r="34" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K34">
+      <c r="K34" s="18">
         <v>0.17033000000000001</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="18">
         <v>8.072E-2</v>
       </c>
-      <c r="AW34">
+      <c r="M34">
+        <v>0.27886</v>
+      </c>
+      <c r="N34">
+        <v>9.6320000000000003E-2</v>
+      </c>
+      <c r="AW34" s="18">
         <v>0.49419999999999997</v>
       </c>
-      <c r="AX34">
+      <c r="AX34" s="18">
         <v>4.1390000000000003E-2</v>
       </c>
       <c r="AZ34">
@@ -24836,16 +26642,22 @@
       </c>
     </row>
     <row r="35" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K35">
+      <c r="K35" s="18">
         <v>0.14645</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="18">
         <v>7.5389999999999999E-2</v>
       </c>
-      <c r="AW35">
+      <c r="M35">
+        <v>0.25</v>
+      </c>
+      <c r="N35">
+        <v>9.3390000000000001E-2</v>
+      </c>
+      <c r="AW35" s="18">
         <v>0.48161999999999999</v>
       </c>
-      <c r="AX35">
+      <c r="AX35" s="18">
         <v>4.2079999999999999E-2</v>
       </c>
       <c r="AZ35">
@@ -24858,16 +26670,22 @@
       </c>
     </row>
     <row r="36" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K36">
+      <c r="K36" s="18">
         <v>0.12408</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="18">
         <v>6.9629999999999997E-2</v>
       </c>
-      <c r="AW36">
+      <c r="M36">
+        <v>0.22220999999999999</v>
+      </c>
+      <c r="N36">
+        <v>8.9779999999999999E-2</v>
+      </c>
+      <c r="AW36" s="18">
         <v>0.46904000000000001</v>
       </c>
-      <c r="AX36">
+      <c r="AX36" s="18">
         <v>4.274E-2</v>
       </c>
       <c r="AZ36">
@@ -24880,16 +26698,22 @@
       </c>
     </row>
     <row r="37" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K37">
+      <c r="K37" s="18">
         <v>0.10332</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="18">
         <v>6.3450000000000006E-2</v>
       </c>
-      <c r="AW37">
+      <c r="M37">
+        <v>0.19561999999999999</v>
+      </c>
+      <c r="N37">
+        <v>8.5529999999999995E-2</v>
+      </c>
+      <c r="AW37" s="18">
         <v>0.43131999999999998</v>
       </c>
-      <c r="AX37">
+      <c r="AX37" s="18">
         <v>4.453E-2</v>
       </c>
       <c r="AZ37">
@@ -24902,16 +26726,22 @@
       </c>
     </row>
     <row r="38" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K38">
+      <c r="K38" s="18">
         <v>8.4269999999999998E-2</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="18">
         <v>5.6910000000000002E-2</v>
       </c>
-      <c r="AW38">
+      <c r="M38">
+        <v>0.17033000000000001</v>
+      </c>
+      <c r="N38">
+        <v>8.072E-2</v>
+      </c>
+      <c r="AW38" s="18">
         <v>0.40620000000000001</v>
       </c>
-      <c r="AX38">
+      <c r="AX38" s="18">
         <v>4.5560000000000003E-2</v>
       </c>
       <c r="AZ38">
@@ -24924,16 +26754,22 @@
       </c>
     </row>
     <row r="39" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K39">
+      <c r="K39" s="18">
         <v>6.6989999999999994E-2</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="18">
         <v>5.0169999999999999E-2</v>
       </c>
-      <c r="AW39">
+      <c r="M39">
+        <v>0.14645</v>
+      </c>
+      <c r="N39">
+        <v>7.5389999999999999E-2</v>
+      </c>
+      <c r="AW39" s="18">
         <v>0.38107999999999997</v>
       </c>
-      <c r="AX39">
+      <c r="AX39" s="18">
         <v>4.6440000000000002E-2</v>
       </c>
       <c r="AZ39">
@@ -24946,16 +26782,22 @@
       </c>
     </row>
     <row r="40" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K40">
+      <c r="K40" s="18">
         <v>5.1560000000000002E-2</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="18">
         <v>4.3180000000000003E-2</v>
       </c>
-      <c r="AW40">
+      <c r="M40">
+        <v>0.13136200000000001</v>
+      </c>
+      <c r="N40">
+        <v>7.1596000000000007E-2</v>
+      </c>
+      <c r="AW40" s="18">
         <v>0.36853000000000002</v>
       </c>
-      <c r="AX40">
+      <c r="AX40" s="18">
         <v>4.6820000000000001E-2</v>
       </c>
       <c r="AZ40">
@@ -24968,16 +26810,22 @@
       </c>
     </row>
     <row r="41" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K41">
+      <c r="K41" s="18">
         <v>3.8059999999999997E-2</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="18">
         <v>3.5749999999999997E-2</v>
       </c>
-      <c r="AW41">
+      <c r="M41">
+        <v>0.12408</v>
+      </c>
+      <c r="N41">
+        <v>6.9629999999999997E-2</v>
+      </c>
+      <c r="AW41" s="18">
         <v>0.35598999999999997</v>
       </c>
-      <c r="AX41">
+      <c r="AX41" s="18">
         <v>4.7160000000000001E-2</v>
       </c>
       <c r="AZ41">
@@ -24990,16 +26838,22 @@
       </c>
     </row>
     <row r="42" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K42">
+      <c r="K42" s="18">
         <v>2.6530000000000001E-2</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="18">
         <v>2.8969999999999999E-2</v>
       </c>
-      <c r="AW42">
+      <c r="M42">
+        <v>0.116976</v>
+      </c>
+      <c r="N42">
+        <v>6.7615999999999996E-2</v>
+      </c>
+      <c r="AW42" s="18">
         <v>0.34345999999999999</v>
       </c>
-      <c r="AX42">
+      <c r="AX42" s="18">
         <v>4.7449999999999999E-2</v>
       </c>
       <c r="AZ42">
@@ -25012,16 +26866,22 @@
       </c>
     </row>
     <row r="43" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K43">
+      <c r="K43" s="18">
         <v>1.704E-2</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="18">
         <v>2.2009999999999998E-2</v>
       </c>
-      <c r="AW43">
+      <c r="M43">
+        <v>0.110054</v>
+      </c>
+      <c r="N43">
+        <v>6.5555000000000002E-2</v>
+      </c>
+      <c r="AW43" s="18">
         <v>0.33093</v>
       </c>
-      <c r="AX43">
+      <c r="AX43" s="18">
         <v>4.7699999999999999E-2</v>
       </c>
       <c r="AZ43">
@@ -25034,16 +26894,22 @@
       </c>
     </row>
     <row r="44" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K44">
+      <c r="K44" s="18">
         <v>9.6100000000000005E-3</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="18">
         <v>1.4239999999999999E-2</v>
       </c>
-      <c r="AW44">
+      <c r="M44">
+        <v>0.10332</v>
+      </c>
+      <c r="N44">
+        <v>6.3450000000000006E-2</v>
+      </c>
+      <c r="AW44" s="18">
         <v>0.29342000000000001</v>
       </c>
-      <c r="AX44">
+      <c r="AX44" s="18">
         <v>4.8140000000000002E-2</v>
       </c>
       <c r="AZ44">
@@ -25056,16 +26922,22 @@
       </c>
     </row>
     <row r="45" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K45">
+      <c r="K45" s="18">
         <v>4.28E-3</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="18">
         <v>7.8399999999999997E-3</v>
       </c>
-      <c r="AW45">
+      <c r="M45">
+        <v>9.6777000000000002E-2</v>
+      </c>
+      <c r="N45">
+        <v>6.1303000000000003E-2</v>
+      </c>
+      <c r="AW45" s="18">
         <v>0.26848</v>
       </c>
-      <c r="AX45">
+      <c r="AX45" s="18">
         <v>4.8160000000000001E-2</v>
       </c>
       <c r="AZ45">
@@ -25078,16 +26950,22 @@
       </c>
     </row>
     <row r="46" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K46">
+      <c r="K46" s="18">
         <v>1.07E-3</v>
       </c>
-      <c r="L46">
+      <c r="L46" s="18">
         <v>3.5300000000000002E-3</v>
       </c>
-      <c r="AW46">
+      <c r="M46">
+        <v>9.0426000000000006E-2</v>
+      </c>
+      <c r="N46">
+        <v>5.9119999999999999E-2</v>
+      </c>
+      <c r="AW46" s="18">
         <v>0.25603999999999999</v>
       </c>
-      <c r="AX46">
+      <c r="AX46" s="18">
         <v>4.8070000000000002E-2</v>
       </c>
       <c r="AZ46">
@@ -25100,16 +26978,22 @@
       </c>
     </row>
     <row r="47" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K47">
+      <c r="K47" s="18">
         <v>0</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="18">
         <v>0</v>
       </c>
-      <c r="AW47">
+      <c r="M47">
+        <v>8.4269999999999998E-2</v>
+      </c>
+      <c r="N47">
+        <v>5.6910000000000002E-2</v>
+      </c>
+      <c r="AW47" s="18">
         <v>0.24362</v>
       </c>
-      <c r="AX47">
+      <c r="AX47" s="18">
         <v>4.7910000000000001E-2</v>
       </c>
       <c r="AZ47">
@@ -25122,14 +27006,18 @@
       </c>
     </row>
     <row r="48" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K48" s="4">
+      <c r="K48" s="19">
         <v>1.07E-3</v>
       </c>
-      <c r="L48" s="4">
+      <c r="L48" s="19">
         <v>-5.1999999999999998E-3</v>
       </c>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
+      <c r="M48" s="4">
+        <v>7.8311000000000006E-2</v>
+      </c>
+      <c r="N48" s="4">
+        <v>5.4678999999999998E-2</v>
+      </c>
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="4"/>
@@ -25142,10 +27030,10 @@
       <c r="X48" s="4"/>
       <c r="Y48" s="4"/>
       <c r="Z48" s="4"/>
-      <c r="AW48">
+      <c r="AW48" s="18">
         <v>0.23122000000000001</v>
       </c>
-      <c r="AX48">
+      <c r="AX48" s="18">
         <v>4.7669999999999997E-2</v>
       </c>
       <c r="AZ48">
@@ -25158,16 +27046,22 @@
       </c>
     </row>
     <row r="49" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K49">
+      <c r="K49" s="18">
         <v>4.28E-3</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="18">
         <v>-8.8199999999999997E-3</v>
       </c>
-      <c r="AW49">
+      <c r="M49">
+        <v>7.2548000000000001E-2</v>
+      </c>
+      <c r="N49">
+        <v>5.2430999999999998E-2</v>
+      </c>
+      <c r="AW49" s="18">
         <v>0.21884999999999999</v>
       </c>
-      <c r="AX49">
+      <c r="AX49" s="18">
         <v>4.7359999999999999E-2</v>
       </c>
       <c r="AZ49">
@@ -25180,16 +27074,22 @@
       </c>
     </row>
     <row r="50" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K50">
+      <c r="K50" s="18">
         <v>9.6100000000000005E-3</v>
       </c>
-      <c r="L50">
+      <c r="L50" s="18">
         <v>-1.205E-2</v>
       </c>
-      <c r="AW50">
+      <c r="M50">
+        <v>6.6989999999999994E-2</v>
+      </c>
+      <c r="N50">
+        <v>5.0169999999999999E-2</v>
+      </c>
+      <c r="AW50" s="18">
         <v>0.20652000000000001</v>
       </c>
-      <c r="AX50">
+      <c r="AX50" s="18">
         <v>4.6960000000000002E-2</v>
       </c>
       <c r="AZ50">
@@ -25202,16 +27102,22 @@
       </c>
     </row>
     <row r="51" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K51">
+      <c r="K51" s="18">
         <v>1.704E-2</v>
       </c>
-      <c r="L51">
+      <c r="L51" s="18">
         <v>-1.502E-2</v>
       </c>
-      <c r="AW51">
+      <c r="M51">
+        <v>6.1636999999999997E-2</v>
+      </c>
+      <c r="N51">
+        <v>4.7892999999999998E-2</v>
+      </c>
+      <c r="AW51" s="18">
         <v>0.15762000000000001</v>
       </c>
-      <c r="AX51">
+      <c r="AX51" s="18">
         <v>4.4339999999999997E-2</v>
       </c>
       <c r="AZ51">
@@ -25224,16 +27130,22 @@
       </c>
     </row>
     <row r="52" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K52">
+      <c r="K52" s="18">
         <v>2.6530000000000001E-2</v>
       </c>
-      <c r="L52">
+      <c r="L52" s="18">
         <v>-1.7999999999999999E-2</v>
       </c>
-      <c r="AW52">
+      <c r="M52">
+        <v>5.6492000000000001E-2</v>
+      </c>
+      <c r="N52">
+        <v>4.5573000000000002E-2</v>
+      </c>
+      <c r="AW52" s="18">
         <v>0.14554</v>
       </c>
-      <c r="AX52">
+      <c r="AX52" s="18">
         <v>4.3380000000000002E-2</v>
       </c>
       <c r="AZ52">
@@ -25246,16 +27158,22 @@
       </c>
     </row>
     <row r="53" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K53">
+      <c r="K53" s="18">
         <v>3.8059999999999997E-2</v>
       </c>
-      <c r="L53">
+      <c r="L53" s="18">
         <v>-2.0619999999999999E-2</v>
       </c>
-      <c r="AW53">
+      <c r="M53">
+        <v>5.1560000000000002E-2</v>
+      </c>
+      <c r="N53">
+        <v>4.3180000000000003E-2</v>
+      </c>
+      <c r="AW53" s="18">
         <v>0.13355</v>
       </c>
-      <c r="AX53">
+      <c r="AX53" s="18">
         <v>4.2290000000000001E-2</v>
       </c>
       <c r="AZ53">
@@ -25268,16 +27186,22 @@
       </c>
     </row>
     <row r="54" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K54">
+      <c r="K54" s="18">
         <v>5.1560000000000002E-2</v>
       </c>
-      <c r="L54">
+      <c r="L54" s="18">
         <v>-2.2370000000000001E-2</v>
       </c>
-      <c r="AW54">
+      <c r="M54">
+        <v>4.6843999999999997E-2</v>
+      </c>
+      <c r="N54">
+        <v>4.07E-2</v>
+      </c>
+      <c r="AW54" s="18">
         <v>0.12166</v>
       </c>
-      <c r="AX54">
+      <c r="AX54" s="18">
         <v>4.1029999999999997E-2</v>
       </c>
       <c r="AZ54">
@@ -25290,16 +27214,22 @@
       </c>
     </row>
     <row r="55" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K55">
+      <c r="K55" s="18">
         <v>6.6989999999999994E-2</v>
       </c>
-      <c r="L55">
+      <c r="L55" s="18">
         <v>-2.4060000000000002E-2</v>
       </c>
-      <c r="AW55">
+      <c r="M55">
+        <v>3.8059999999999997E-2</v>
+      </c>
+      <c r="N55">
+        <v>3.5749999999999997E-2</v>
+      </c>
+      <c r="AW55" s="18">
         <v>9.8250000000000004E-2</v>
       </c>
-      <c r="AX55">
+      <c r="AX55" s="18">
         <v>3.8010000000000002E-2</v>
       </c>
       <c r="AZ55">
@@ -25312,16 +27242,22 @@
       </c>
     </row>
     <row r="56" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K56">
+      <c r="K56" s="18">
         <v>8.4269999999999998E-2</v>
       </c>
-      <c r="L56">
+      <c r="L56" s="18">
         <v>-2.5239999999999999E-2</v>
       </c>
-      <c r="AW56">
+      <c r="M56">
+        <v>3.0148999999999999E-2</v>
+      </c>
+      <c r="N56">
+        <v>3.1178000000000001E-2</v>
+      </c>
+      <c r="AW56" s="18">
         <v>7.5560000000000002E-2</v>
       </c>
-      <c r="AX56">
+      <c r="AX56" s="18">
         <v>3.415E-2</v>
       </c>
       <c r="AZ56">
@@ -25334,16 +27270,22 @@
       </c>
     </row>
     <row r="57" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K57">
+      <c r="K57" s="18">
         <v>0.10332</v>
       </c>
-      <c r="L57">
+      <c r="L57" s="18">
         <v>-2.598E-2</v>
       </c>
-      <c r="AW57">
+      <c r="M57">
+        <v>2.6530000000000001E-2</v>
+      </c>
+      <c r="N57">
+        <v>2.8969999999999999E-2</v>
+      </c>
+      <c r="AW57" s="18">
         <v>6.4600000000000005E-2</v>
       </c>
-      <c r="AX57">
+      <c r="AX57" s="18">
         <v>3.1859999999999999E-2</v>
       </c>
       <c r="AZ57">
@@ -25356,16 +27298,22 @@
       </c>
     </row>
     <row r="58" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K58">
+      <c r="K58" s="18">
         <v>0.12408</v>
       </c>
-      <c r="L58">
+      <c r="L58" s="18">
         <v>-2.6419999999999999E-2</v>
       </c>
-      <c r="AW58">
+      <c r="M58">
+        <v>2.3139E-2</v>
+      </c>
+      <c r="N58">
+        <v>2.6741999999999998E-2</v>
+      </c>
+      <c r="AW58" s="18">
         <v>3.4520000000000002E-2</v>
       </c>
-      <c r="AX58">
+      <c r="AX58" s="18">
         <v>2.3470000000000001E-2</v>
       </c>
       <c r="AZ58">
@@ -25378,16 +27326,22 @@
       </c>
     </row>
     <row r="59" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K59">
+      <c r="K59" s="18">
         <v>0.14645</v>
       </c>
-      <c r="L59">
+      <c r="L59" s="18">
         <v>-2.6530000000000001E-2</v>
       </c>
-      <c r="AW59">
+      <c r="M59">
+        <v>1.9975E-2</v>
+      </c>
+      <c r="N59">
+        <v>2.444E-2</v>
+      </c>
+      <c r="AW59" s="18">
         <v>2.6190000000000001E-2</v>
       </c>
-      <c r="AX59">
+      <c r="AX59" s="18">
         <v>2.0299999999999999E-2</v>
       </c>
       <c r="AZ59">
@@ -25400,16 +27354,22 @@
       </c>
     </row>
     <row r="60" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K60">
+      <c r="K60" s="18">
         <v>0.17033000000000001</v>
       </c>
-      <c r="L60">
+      <c r="L60" s="18">
         <v>-2.631E-2</v>
       </c>
-      <c r="AW60">
+      <c r="M60">
+        <v>1.704E-2</v>
+      </c>
+      <c r="N60">
+        <v>2.2009999999999998E-2</v>
+      </c>
+      <c r="AW60" s="18">
         <v>1.925E-2</v>
       </c>
-      <c r="AX60">
+      <c r="AX60" s="18">
         <v>1.7180000000000001E-2</v>
       </c>
       <c r="AZ60">
@@ -25422,16 +27382,22 @@
       </c>
     </row>
     <row r="61" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K61">
+      <c r="K61" s="18">
         <v>0.19561999999999999</v>
       </c>
-      <c r="L61">
+      <c r="L61" s="18">
         <v>-2.5839999999999998E-2</v>
       </c>
-      <c r="AW61">
+      <c r="M61">
+        <v>1.4333E-2</v>
+      </c>
+      <c r="N61">
+        <v>1.9428000000000001E-2</v>
+      </c>
+      <c r="AW61" s="18">
         <v>1.384E-2</v>
       </c>
-      <c r="AX61">
+      <c r="AX61" s="18">
         <v>1.43E-2</v>
       </c>
       <c r="AZ61">
@@ -25444,16 +27410,22 @@
       </c>
     </row>
     <row r="62" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K62">
+      <c r="K62" s="18">
         <v>0.22220999999999999</v>
       </c>
-      <c r="L62">
+      <c r="L62" s="18">
         <v>-2.512E-2</v>
       </c>
-      <c r="AW62">
+      <c r="M62">
+        <v>1.1854999999999999E-2</v>
+      </c>
+      <c r="N62">
+        <v>1.6794E-2</v>
+      </c>
+      <c r="AW62" s="18">
         <v>6.8100000000000001E-3</v>
       </c>
-      <c r="AX62">
+      <c r="AX62" s="18">
         <v>9.5600000000000008E-3</v>
       </c>
       <c r="AZ62">
@@ -25466,16 +27438,22 @@
       </c>
     </row>
     <row r="63" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K63">
+      <c r="K63" s="18">
         <v>0.25</v>
       </c>
-      <c r="L63">
+      <c r="L63" s="18">
         <v>-2.419E-2</v>
       </c>
-      <c r="AW63">
+      <c r="M63">
+        <v>9.6100000000000005E-3</v>
+      </c>
+      <c r="N63">
+        <v>1.4239999999999999E-2</v>
+      </c>
+      <c r="AW63" s="18">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="AX63">
+      <c r="AX63" s="18">
         <v>7.6299999999999996E-3</v>
       </c>
       <c r="AZ63">
@@ -25488,16 +27466,22 @@
       </c>
     </row>
     <row r="64" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K64">
+      <c r="K64" s="18">
         <v>0.27886</v>
       </c>
-      <c r="L64">
+      <c r="L64" s="18">
         <v>-2.308E-2</v>
       </c>
-      <c r="AW64">
+      <c r="M64">
+        <v>7.5989999999999999E-3</v>
+      </c>
+      <c r="N64">
+        <v>1.1877E-2</v>
+      </c>
+      <c r="AW64" s="18">
         <v>1.74E-3</v>
       </c>
-      <c r="AX64">
+      <c r="AX64" s="18">
         <v>4.3499999999999997E-3</v>
       </c>
       <c r="AZ64">
@@ -25510,16 +27494,22 @@
       </c>
     </row>
     <row r="65" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K65">
+      <c r="K65" s="18">
         <v>0.30865999999999999</v>
       </c>
-      <c r="L65">
+      <c r="L65" s="18">
         <v>-2.1839999999999998E-2</v>
       </c>
-      <c r="AW65">
+      <c r="M65">
+        <v>5.8219999999999999E-3</v>
+      </c>
+      <c r="N65">
+        <v>9.7389999999999994E-3</v>
+      </c>
+      <c r="AW65" s="18">
         <v>2.7999999999999998E-4</v>
       </c>
-      <c r="AX65">
+      <c r="AX65" s="18">
         <v>1.6100000000000001E-3</v>
       </c>
       <c r="AZ65">
@@ -25532,16 +27522,22 @@
       </c>
     </row>
     <row r="66" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K66">
+      <c r="K66" s="18">
         <v>0.33928000000000003</v>
       </c>
-      <c r="L66">
+      <c r="L66" s="18">
         <v>-2.0469999999999999E-2</v>
       </c>
-      <c r="AW66">
+      <c r="M66">
+        <v>4.28E-3</v>
+      </c>
+      <c r="N66">
+        <v>7.8399999999999997E-3</v>
+      </c>
+      <c r="AW66" s="18">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AX66">
+      <c r="AX66" s="18">
         <v>3.8000000000000002E-4</v>
       </c>
       <c r="AZ66">
@@ -25554,16 +27550,22 @@
       </c>
     </row>
     <row r="67" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K67">
+      <c r="K67" s="18">
         <v>0.37058999999999997</v>
       </c>
-      <c r="L67">
+      <c r="L67" s="18">
         <v>-1.9040000000000001E-2</v>
       </c>
-      <c r="AW67">
+      <c r="M67">
+        <v>2.9729999999999999E-3</v>
+      </c>
+      <c r="N67">
+        <v>6.1869999999999998E-3</v>
+      </c>
+      <c r="AW67" s="18">
         <v>0</v>
       </c>
-      <c r="AX67">
+      <c r="AX67" s="18">
         <v>0</v>
       </c>
       <c r="AZ67">
@@ -25576,16 +27578,22 @@
       </c>
     </row>
     <row r="68" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K68">
+      <c r="K68" s="18">
         <v>0.40244999999999997</v>
       </c>
-      <c r="L68">
+      <c r="L68" s="18">
         <v>-1.754E-2</v>
       </c>
-      <c r="AW68" s="4">
+      <c r="M68">
+        <v>1.903E-3</v>
+      </c>
+      <c r="N68">
+        <v>4.7590000000000002E-3</v>
+      </c>
+      <c r="AW68" s="19">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AX68" s="4">
+      <c r="AX68" s="19">
         <v>-3.8000000000000002E-4</v>
       </c>
       <c r="AZ68">
@@ -25598,16 +27606,22 @@
       </c>
     </row>
     <row r="69" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K69">
+      <c r="K69" s="18">
         <v>0.43474000000000002</v>
       </c>
-      <c r="L69">
+      <c r="L69" s="18">
         <v>-1.602E-2</v>
       </c>
-      <c r="AW69">
+      <c r="M69">
+        <v>1.07E-3</v>
+      </c>
+      <c r="N69">
+        <v>3.5300000000000002E-3</v>
+      </c>
+      <c r="AW69" s="18">
         <v>2.7999999999999998E-4</v>
       </c>
-      <c r="AX69">
+      <c r="AX69" s="18">
         <v>-1.6100000000000001E-3</v>
       </c>
       <c r="AZ69">
@@ -25620,16 +27634,22 @@
       </c>
     </row>
     <row r="70" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K70">
+      <c r="K70" s="18">
         <v>0.46729999999999999</v>
       </c>
-      <c r="L70">
+      <c r="L70" s="18">
         <v>-1.451E-2</v>
       </c>
-      <c r="AW70">
+      <c r="M70">
+        <v>4.75E-4</v>
+      </c>
+      <c r="N70">
+        <v>2.4429999999999999E-3</v>
+      </c>
+      <c r="AW70" s="18">
         <v>1.74E-3</v>
       </c>
-      <c r="AX70">
+      <c r="AX70" s="18">
         <v>-4.3499999999999997E-3</v>
       </c>
       <c r="AZ70">
@@ -25642,16 +27662,22 @@
       </c>
     </row>
     <row r="71" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K71">
+      <c r="K71" s="18">
         <v>0.5</v>
       </c>
-      <c r="L71">
+      <c r="L71" s="18">
         <v>-1.3010000000000001E-2</v>
       </c>
-      <c r="AW71">
+      <c r="M71">
+        <v>1.1900000000000001E-4</v>
+      </c>
+      <c r="N71">
+        <v>1.3320000000000001E-3</v>
+      </c>
+      <c r="AW71" s="18">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="AX71">
+      <c r="AX71" s="18">
         <v>-7.6299999999999996E-3</v>
       </c>
       <c r="AZ71">
@@ -25664,16 +27690,22 @@
       </c>
     </row>
     <row r="72" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K72">
+      <c r="K72" s="18">
         <v>0.53269999999999995</v>
       </c>
-      <c r="L72">
+      <c r="L72" s="18">
         <v>-1.1560000000000001E-2</v>
       </c>
-      <c r="AW72">
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="AW72" s="18">
         <v>6.8100000000000001E-3</v>
       </c>
-      <c r="AX72">
+      <c r="AX72" s="18">
         <v>-9.5600000000000008E-3</v>
       </c>
       <c r="AZ72">
@@ -25686,16 +27718,22 @@
       </c>
     </row>
     <row r="73" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K73">
+      <c r="K73" s="18">
         <v>0.56525999999999998</v>
       </c>
-      <c r="L73">
+      <c r="L73" s="18">
         <v>-1.017E-2</v>
       </c>
-      <c r="AW73">
+      <c r="M73">
+        <v>1.1900000000000001E-4</v>
+      </c>
+      <c r="N73">
+        <v>-1.67E-3</v>
+      </c>
+      <c r="AW73" s="18">
         <v>1.384E-2</v>
       </c>
-      <c r="AX73">
+      <c r="AX73" s="18">
         <v>-1.43E-2</v>
       </c>
       <c r="AZ73">
@@ -25708,16 +27746,22 @@
       </c>
     </row>
     <row r="74" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K74">
+      <c r="K74" s="18">
         <v>0.59755000000000003</v>
       </c>
-      <c r="L74">
+      <c r="L74" s="18">
         <v>-8.8500000000000002E-3</v>
       </c>
-      <c r="AW74">
+      <c r="M74">
+        <v>4.75E-4</v>
+      </c>
+      <c r="N74">
+        <v>-3.4919999999999999E-3</v>
+      </c>
+      <c r="AW74" s="18">
         <v>1.925E-2</v>
       </c>
-      <c r="AX74">
+      <c r="AX74" s="18">
         <v>-1.7180000000000001E-2</v>
       </c>
       <c r="AZ74">
@@ -25730,16 +27774,22 @@
       </c>
     </row>
     <row r="75" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K75">
+      <c r="K75" s="18">
         <v>0.62941000000000003</v>
       </c>
-      <c r="L75">
+      <c r="L75" s="18">
         <v>-7.6099999999999996E-3</v>
       </c>
-      <c r="AW75">
+      <c r="M75">
+        <v>1.07E-3</v>
+      </c>
+      <c r="N75">
+        <v>-5.1999999999999998E-3</v>
+      </c>
+      <c r="AW75" s="18">
         <v>2.6190000000000001E-2</v>
       </c>
-      <c r="AX75">
+      <c r="AX75" s="18">
         <v>-2.0299999999999999E-2</v>
       </c>
       <c r="AZ75">
@@ -25752,16 +27802,22 @@
       </c>
     </row>
     <row r="76" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K76">
+      <c r="K76" s="18">
         <v>0.66071999999999997</v>
       </c>
-      <c r="L76">
+      <c r="L76" s="18">
         <v>-6.4599999999999996E-3</v>
       </c>
-      <c r="AW76">
+      <c r="M76">
+        <v>1.903E-3</v>
+      </c>
+      <c r="N76">
+        <v>-6.5970000000000004E-3</v>
+      </c>
+      <c r="AW76" s="18">
         <v>3.4520000000000002E-2</v>
       </c>
-      <c r="AX76">
+      <c r="AX76" s="18">
         <v>-2.3470000000000001E-2</v>
       </c>
       <c r="AZ76">
@@ -25774,16 +27830,22 @@
       </c>
     </row>
     <row r="77" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K77">
+      <c r="K77" s="18">
         <v>0.69133999999999995</v>
       </c>
-      <c r="L77">
+      <c r="L77" s="18">
         <v>-5.4200000000000003E-3</v>
       </c>
-      <c r="AW77">
+      <c r="M77">
+        <v>2.9729999999999999E-3</v>
+      </c>
+      <c r="N77">
+        <v>-7.757E-3</v>
+      </c>
+      <c r="AW77" s="18">
         <v>6.4600000000000005E-2</v>
       </c>
-      <c r="AX77">
+      <c r="AX77" s="18">
         <v>-3.1859999999999999E-2</v>
       </c>
       <c r="AZ77">
@@ -25796,16 +27858,22 @@
       </c>
     </row>
     <row r="78" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K78">
+      <c r="K78" s="18">
         <v>0.72114</v>
       </c>
-      <c r="L78">
+      <c r="L78" s="18">
         <v>-4.4799999999999996E-3</v>
       </c>
-      <c r="AW78">
+      <c r="M78">
+        <v>4.28E-3</v>
+      </c>
+      <c r="N78">
+        <v>-8.8199999999999997E-3</v>
+      </c>
+      <c r="AW78" s="18">
         <v>7.5560000000000002E-2</v>
       </c>
-      <c r="AX78">
+      <c r="AX78" s="18">
         <v>-3.415E-2</v>
       </c>
       <c r="AZ78">
@@ -25818,16 +27886,22 @@
       </c>
     </row>
     <row r="79" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K79">
+      <c r="K79" s="18">
         <v>0.75</v>
       </c>
-      <c r="L79">
+      <c r="L79" s="18">
         <v>-3.64E-3</v>
       </c>
-      <c r="AW79">
+      <c r="M79">
+        <v>5.8219999999999999E-3</v>
+      </c>
+      <c r="N79">
+        <v>-9.8989999999999998E-3</v>
+      </c>
+      <c r="AW79" s="18">
         <v>9.8250000000000004E-2</v>
       </c>
-      <c r="AX79">
+      <c r="AX79" s="18">
         <v>-3.8010000000000002E-2</v>
       </c>
       <c r="AZ79">
@@ -25840,16 +27914,22 @@
       </c>
     </row>
     <row r="80" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K80">
+      <c r="K80" s="18">
         <v>0.77778999999999998</v>
       </c>
-      <c r="L80">
+      <c r="L80" s="18">
         <v>-2.9099999999999998E-3</v>
       </c>
-      <c r="AW80">
+      <c r="M80">
+        <v>7.5989999999999999E-3</v>
+      </c>
+      <c r="N80">
+        <v>-1.0987E-2</v>
+      </c>
+      <c r="AW80" s="18">
         <v>0.12166</v>
       </c>
-      <c r="AX80">
+      <c r="AX80" s="18">
         <v>-4.1029999999999997E-2</v>
       </c>
       <c r="AZ80">
@@ -25862,16 +27942,22 @@
       </c>
     </row>
     <row r="81" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K81">
+      <c r="K81" s="18">
         <v>0.80437999999999998</v>
       </c>
-      <c r="L81">
+      <c r="L81" s="18">
         <v>-2.2699999999999999E-3</v>
       </c>
-      <c r="AW81">
+      <c r="M81">
+        <v>9.6100000000000005E-3</v>
+      </c>
+      <c r="N81">
+        <v>-1.205E-2</v>
+      </c>
+      <c r="AW81" s="18">
         <v>0.13355</v>
       </c>
-      <c r="AX81">
+      <c r="AX81" s="18">
         <v>-4.2290000000000001E-2</v>
       </c>
       <c r="AZ81">
@@ -25884,16 +27970,22 @@
       </c>
     </row>
     <row r="82" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K82">
+      <c r="K82" s="18">
         <v>0.82004999999999995</v>
       </c>
-      <c r="L82">
+      <c r="L82" s="18">
         <v>-1.9400000000000001E-3</v>
       </c>
-      <c r="AW82">
+      <c r="M82">
+        <v>1.1854999999999999E-2</v>
+      </c>
+      <c r="N82">
+        <v>-1.3063E-2</v>
+      </c>
+      <c r="AW82" s="18">
         <v>0.14554</v>
       </c>
-      <c r="AX82">
+      <c r="AX82" s="18">
         <v>-4.3380000000000002E-2</v>
       </c>
       <c r="AZ82">
@@ -25906,16 +27998,22 @@
       </c>
     </row>
     <row r="83" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K83">
+      <c r="K83" s="18">
         <v>0.89553000000000005</v>
       </c>
-      <c r="L83">
+      <c r="L83" s="18">
         <v>2.5500000000000002E-3</v>
       </c>
-      <c r="AW83">
+      <c r="M83">
+        <v>1.4333E-2</v>
+      </c>
+      <c r="N83">
+        <v>-1.4043999999999999E-2</v>
+      </c>
+      <c r="AW83" s="18">
         <v>0.15762000000000001</v>
       </c>
-      <c r="AX83">
+      <c r="AX83" s="18">
         <v>-4.4339999999999997E-2</v>
       </c>
       <c r="AZ83">
@@ -25928,16 +28026,22 @@
       </c>
     </row>
     <row r="84" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K84">
+      <c r="K84" s="18">
         <v>0.95184000000000002</v>
       </c>
-      <c r="L84">
+      <c r="L84" s="18">
         <v>9.0799999999999995E-3</v>
       </c>
-      <c r="AW84">
+      <c r="M84">
+        <v>1.704E-2</v>
+      </c>
+      <c r="N84">
+        <v>-1.502E-2</v>
+      </c>
+      <c r="AW84" s="18">
         <v>0.20652000000000001</v>
       </c>
-      <c r="AX84">
+      <c r="AX84" s="18">
         <v>-4.6960000000000002E-2</v>
       </c>
       <c r="AZ84">
@@ -25950,16 +28054,22 @@
       </c>
     </row>
     <row r="85" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K85">
+      <c r="K85" s="18">
         <v>0.98662000000000005</v>
       </c>
-      <c r="L85">
+      <c r="L85" s="18">
         <v>1.4109999999999999E-2</v>
       </c>
-      <c r="AW85">
+      <c r="M85">
+        <v>1.9975E-2</v>
+      </c>
+      <c r="N85">
+        <v>-1.6012999999999999E-2</v>
+      </c>
+      <c r="AW85" s="18">
         <v>0.21884999999999999</v>
       </c>
-      <c r="AX85">
+      <c r="AX85" s="18">
         <v>-4.7359999999999999E-2</v>
       </c>
       <c r="AZ85">
@@ -25972,16 +28082,22 @@
       </c>
     </row>
     <row r="86" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="K86">
+      <c r="K86" s="18">
         <v>0.99839</v>
       </c>
-      <c r="L86">
+      <c r="L86" s="18">
         <v>1.5949999999999999E-2</v>
       </c>
-      <c r="AW86">
+      <c r="M86">
+        <v>2.3139E-2</v>
+      </c>
+      <c r="N86">
+        <v>-1.7011999999999999E-2</v>
+      </c>
+      <c r="AW86" s="18">
         <v>0.23122000000000001</v>
       </c>
-      <c r="AX86">
+      <c r="AX86" s="18">
         <v>-4.7669999999999997E-2</v>
       </c>
       <c r="AZ86">
@@ -25994,322 +28110,562 @@
       </c>
     </row>
     <row r="87" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="AW87">
+      <c r="M87">
+        <v>2.6530000000000001E-2</v>
+      </c>
+      <c r="N87">
+        <v>-1.7999999999999999E-2</v>
+      </c>
+      <c r="AW87" s="18">
         <v>0.24362</v>
       </c>
-      <c r="AX87">
+      <c r="AX87" s="18">
         <v>-4.7910000000000001E-2</v>
       </c>
     </row>
     <row r="88" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="AW88">
+      <c r="M88">
+        <v>3.0148999999999999E-2</v>
+      </c>
+      <c r="N88">
+        <v>-1.8956000000000001E-2</v>
+      </c>
+      <c r="AW88" s="18">
         <v>0.25603999999999999</v>
       </c>
-      <c r="AX88">
+      <c r="AX88" s="18">
         <v>-4.8070000000000002E-2</v>
       </c>
     </row>
     <row r="89" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="AW89">
+      <c r="M89">
+        <v>3.3994999999999997E-2</v>
+      </c>
+      <c r="N89">
+        <v>-1.9843E-2</v>
+      </c>
+      <c r="AW89" s="18">
         <v>0.26848</v>
       </c>
-      <c r="AX89">
+      <c r="AX89" s="18">
         <v>-4.8160000000000001E-2</v>
       </c>
     </row>
     <row r="90" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="AW90">
+      <c r="M90">
+        <v>3.8059999999999997E-2</v>
+      </c>
+      <c r="N90">
+        <v>-2.0619999999999999E-2</v>
+      </c>
+      <c r="AW90" s="18">
         <v>0.29342000000000001</v>
       </c>
-      <c r="AX90">
+      <c r="AX90" s="18">
         <v>-4.8140000000000002E-2</v>
       </c>
     </row>
     <row r="91" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="AW91">
+      <c r="M91">
+        <v>4.2342999999999999E-2</v>
+      </c>
+      <c r="N91">
+        <v>-2.1264999999999999E-2</v>
+      </c>
+      <c r="AW91" s="18">
         <v>0.33093</v>
       </c>
-      <c r="AX91">
+      <c r="AX91" s="18">
         <v>-4.7699999999999999E-2</v>
       </c>
     </row>
     <row r="92" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="AW92">
+      <c r="M92">
+        <v>5.1560000000000002E-2</v>
+      </c>
+      <c r="N92">
+        <v>-2.2370000000000001E-2</v>
+      </c>
+      <c r="AW92" s="18">
         <v>0.34345999999999999</v>
       </c>
-      <c r="AX92">
+      <c r="AX92" s="18">
         <v>-4.7449999999999999E-2</v>
       </c>
     </row>
     <row r="93" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="AW93">
+      <c r="M93">
+        <v>6.1636999999999997E-2</v>
+      </c>
+      <c r="N93">
+        <v>-2.3522999999999999E-2</v>
+      </c>
+      <c r="AW93" s="18">
         <v>0.35598999999999997</v>
       </c>
-      <c r="AX93">
+      <c r="AX93" s="18">
         <v>-4.7160000000000001E-2</v>
       </c>
     </row>
     <row r="94" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="AW94">
+      <c r="M94">
+        <v>6.6989999999999994E-2</v>
+      </c>
+      <c r="N94">
+        <v>-2.4060000000000002E-2</v>
+      </c>
+      <c r="AW94" s="18">
         <v>0.36853000000000002</v>
       </c>
-      <c r="AX94">
+      <c r="AX94" s="18">
         <v>-4.6820000000000001E-2</v>
       </c>
     </row>
     <row r="95" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="AW95">
+      <c r="M95">
+        <v>7.2548000000000001E-2</v>
+      </c>
+      <c r="N95">
+        <v>-2.4521000000000001E-2</v>
+      </c>
+      <c r="AW95" s="18">
         <v>0.38107999999999997</v>
       </c>
-      <c r="AX95">
+      <c r="AX95" s="18">
         <v>-4.6440000000000002E-2</v>
       </c>
     </row>
     <row r="96" spans="11:53" x14ac:dyDescent="0.25">
-      <c r="AW96">
+      <c r="M96">
+        <v>8.4269999999999998E-2</v>
+      </c>
+      <c r="N96">
+        <v>-2.5239999999999999E-2</v>
+      </c>
+      <c r="AW96" s="18">
         <v>0.40620000000000001</v>
       </c>
-      <c r="AX96">
+      <c r="AX96" s="18">
         <v>-4.5560000000000003E-2</v>
       </c>
     </row>
-    <row r="97" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW97">
+    <row r="97" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M97">
+        <v>0.10332</v>
+      </c>
+      <c r="N97">
+        <v>-2.598E-2</v>
+      </c>
+      <c r="AW97" s="18">
         <v>0.43131999999999998</v>
       </c>
-      <c r="AX97">
+      <c r="AX97" s="18">
         <v>-4.453E-2</v>
       </c>
     </row>
-    <row r="98" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW98">
+    <row r="98" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M98">
+        <v>0.12408</v>
+      </c>
+      <c r="N98">
+        <v>-2.6419999999999999E-2</v>
+      </c>
+      <c r="AW98" s="18">
         <v>0.46904000000000001</v>
       </c>
-      <c r="AX98">
+      <c r="AX98" s="18">
         <v>-4.274E-2</v>
       </c>
     </row>
-    <row r="99" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW99">
+    <row r="99" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M99">
+        <v>0.14645</v>
+      </c>
+      <c r="N99">
+        <v>-2.6530000000000001E-2</v>
+      </c>
+      <c r="AW99" s="18">
         <v>0.48161999999999999</v>
       </c>
-      <c r="AX99">
+      <c r="AX99" s="18">
         <v>-4.2079999999999999E-2</v>
       </c>
     </row>
-    <row r="100" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW100">
+    <row r="100" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M100">
+        <v>0.17033000000000001</v>
+      </c>
+      <c r="N100">
+        <v>-2.631E-2</v>
+      </c>
+      <c r="AW100" s="18">
         <v>0.49419999999999997</v>
       </c>
-      <c r="AX100">
+      <c r="AX100" s="18">
         <v>-4.1390000000000003E-2</v>
       </c>
     </row>
-    <row r="101" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW101">
+    <row r="101" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M101">
+        <v>0.19561999999999999</v>
+      </c>
+      <c r="N101">
+        <v>-2.5839999999999998E-2</v>
+      </c>
+      <c r="AW101" s="18">
         <v>0.50678000000000001</v>
       </c>
-      <c r="AX101">
+      <c r="AX101" s="18">
         <v>-4.0669999999999998E-2</v>
       </c>
     </row>
-    <row r="102" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW102">
+    <row r="102" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M102">
+        <v>0.22220999999999999</v>
+      </c>
+      <c r="N102">
+        <v>-2.512E-2</v>
+      </c>
+      <c r="AW102" s="18">
         <v>0.54454999999999998</v>
       </c>
-      <c r="AX102">
+      <c r="AX102" s="18">
         <v>-3.8359999999999998E-2</v>
       </c>
     </row>
-    <row r="103" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW103">
+    <row r="103" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M103">
+        <v>0.25</v>
+      </c>
+      <c r="N103">
+        <v>-2.419E-2</v>
+      </c>
+      <c r="AW103" s="18">
         <v>0.55715000000000003</v>
       </c>
-      <c r="AX103">
+      <c r="AX103" s="18">
         <v>-3.7539999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW104">
+    <row r="104" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M104">
+        <v>0.27886</v>
+      </c>
+      <c r="N104">
+        <v>-2.308E-2</v>
+      </c>
+      <c r="AW104" s="18">
         <v>0.56974999999999998</v>
       </c>
-      <c r="AX104">
+      <c r="AX104" s="18">
         <v>-3.6700000000000003E-2</v>
       </c>
     </row>
-    <row r="105" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW105">
+    <row r="105" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M105">
+        <v>0.30865999999999999</v>
+      </c>
+      <c r="N105">
+        <v>-2.1839999999999998E-2</v>
+      </c>
+      <c r="AW105" s="18">
         <v>0.59494999999999998</v>
       </c>
-      <c r="AX105">
+      <c r="AX105" s="18">
         <v>-3.4959999999999998E-2</v>
       </c>
     </row>
-    <row r="106" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW106">
+    <row r="106" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M106">
+        <v>0.40244999999999997</v>
+      </c>
+      <c r="N106">
+        <v>-1.754E-2</v>
+      </c>
+      <c r="AW106" s="18">
         <v>0.60755999999999999</v>
       </c>
-      <c r="AX106">
+      <c r="AX106" s="18">
         <v>-3.406E-2</v>
       </c>
     </row>
-    <row r="107" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW107">
+    <row r="107" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M107">
+        <v>0.46729999999999999</v>
+      </c>
+      <c r="N107">
+        <v>-1.451E-2</v>
+      </c>
+      <c r="AW107" s="18">
         <v>0.62017</v>
       </c>
-      <c r="AX107">
+      <c r="AX107" s="18">
         <v>-3.3149999999999999E-2</v>
       </c>
     </row>
-    <row r="108" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW108">
+    <row r="108" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M108">
+        <v>0.5</v>
+      </c>
+      <c r="N108">
+        <v>-1.3010000000000001E-2</v>
+      </c>
+      <c r="AW108" s="18">
         <v>0.65800999999999998</v>
       </c>
-      <c r="AX108">
+      <c r="AX108" s="18">
         <v>-3.031E-2</v>
       </c>
     </row>
-    <row r="109" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW109">
+    <row r="109" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M109">
+        <v>0.53269999999999995</v>
+      </c>
+      <c r="N109">
+        <v>-1.1560000000000001E-2</v>
+      </c>
+      <c r="AW109" s="18">
         <v>0.67062999999999995</v>
       </c>
-      <c r="AX109">
+      <c r="AX109" s="18">
         <v>-2.9329999999999998E-2</v>
       </c>
     </row>
-    <row r="110" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW110">
+    <row r="110" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M110">
+        <v>0.59755000000000003</v>
+      </c>
+      <c r="N110">
+        <v>-8.8500000000000002E-3</v>
+      </c>
+      <c r="AW110" s="18">
         <v>0.68325000000000002</v>
       </c>
-      <c r="AX110">
+      <c r="AX110" s="18">
         <v>-2.8340000000000001E-2</v>
       </c>
     </row>
-    <row r="111" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW111">
+    <row r="111" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M111">
+        <v>0.62941000000000003</v>
+      </c>
+      <c r="N111">
+        <v>-7.6099999999999996E-3</v>
+      </c>
+      <c r="AW111" s="18">
         <v>0.69586999999999999</v>
       </c>
-      <c r="AX111">
+      <c r="AX111" s="18">
         <v>-2.734E-2</v>
       </c>
     </row>
-    <row r="112" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW112">
+    <row r="112" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M112">
+        <v>0.66071999999999997</v>
+      </c>
+      <c r="N112">
+        <v>-6.4599999999999996E-3</v>
+      </c>
+      <c r="AW112" s="18">
         <v>0.72111999999999998</v>
       </c>
-      <c r="AX112">
+      <c r="AX112" s="18">
         <v>-2.5309999999999999E-2</v>
       </c>
     </row>
-    <row r="113" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW113">
+    <row r="113" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M113">
+        <v>0.69133999999999995</v>
+      </c>
+      <c r="N113">
+        <v>-5.4200000000000003E-3</v>
+      </c>
+      <c r="AW113" s="18">
         <v>0.73373999999999995</v>
       </c>
-      <c r="AX113">
+      <c r="AX113" s="18">
         <v>-2.4279999999999999E-2</v>
       </c>
     </row>
-    <row r="114" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW114">
+    <row r="114" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M114">
+        <v>0.72114</v>
+      </c>
+      <c r="N114">
+        <v>-4.4799999999999996E-3</v>
+      </c>
+      <c r="AW114" s="18">
         <v>0.77159999999999995</v>
       </c>
-      <c r="AX114">
+      <c r="AX114" s="18">
         <v>-2.1129999999999999E-2</v>
       </c>
     </row>
-    <row r="115" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW115">
+    <row r="115" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M115">
+        <v>0.75</v>
+      </c>
+      <c r="N115">
+        <v>-3.64E-3</v>
+      </c>
+      <c r="AW115" s="18">
         <v>0.78422000000000003</v>
       </c>
-      <c r="AX115">
+      <c r="AX115" s="18">
         <v>-2.0060000000000001E-2</v>
       </c>
     </row>
-    <row r="116" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW116">
+    <row r="116" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M116">
+        <v>0.77778999999999998</v>
+      </c>
+      <c r="N116">
+        <v>-2.9099999999999998E-3</v>
+      </c>
+      <c r="AW116" s="18">
         <v>0.79683000000000004</v>
       </c>
-      <c r="AX116">
+      <c r="AX116" s="18">
         <v>-1.898E-2</v>
       </c>
     </row>
-    <row r="117" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW117">
+    <row r="117" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M117">
+        <v>0.80437999999999998</v>
+      </c>
+      <c r="N117">
+        <v>-2.2699999999999999E-3</v>
+      </c>
+      <c r="AW117" s="18">
         <v>0.80944000000000005</v>
       </c>
-      <c r="AX117">
+      <c r="AX117" s="18">
         <v>-1.789E-2</v>
       </c>
     </row>
-    <row r="118" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW118">
+    <row r="118" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M118">
+        <v>0.81008000000000002</v>
+      </c>
+      <c r="N118">
+        <v>-2.3319999999999999E-3</v>
+      </c>
+      <c r="AW118" s="18">
         <v>0.82206000000000001</v>
       </c>
-      <c r="AX118">
+      <c r="AX118" s="18">
         <v>-1.6789999999999999E-2</v>
       </c>
     </row>
-    <row r="119" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW119">
+    <row r="119" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M119">
+        <v>0.82004999999999995</v>
+      </c>
+      <c r="N119">
+        <v>-1.9400000000000001E-3</v>
+      </c>
+      <c r="AW119" s="18">
         <v>0.84728000000000003</v>
       </c>
-      <c r="AX119">
+      <c r="AX119" s="18">
         <v>-1.455E-2</v>
       </c>
     </row>
-    <row r="120" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW120">
+    <row r="120" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M120">
+        <v>0.84077800000000003</v>
+      </c>
+      <c r="N120">
+        <v>-9.2800000000000001E-4</v>
+      </c>
+      <c r="AW120" s="18">
         <v>0.88514999999999999</v>
       </c>
-      <c r="AX120">
+      <c r="AX120" s="18">
         <v>-1.1140000000000001E-2</v>
       </c>
     </row>
-    <row r="121" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW121">
+    <row r="121" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M121">
+        <v>0.86804099999999995</v>
+      </c>
+      <c r="N121">
+        <v>6.2200000000000005E-4</v>
+      </c>
+      <c r="AW121" s="18">
         <v>0.89778000000000002</v>
       </c>
-      <c r="AX121">
+      <c r="AX121" s="18">
         <v>-9.9900000000000006E-3</v>
       </c>
     </row>
-    <row r="122" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW122">
+    <row r="122" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M122">
+        <v>0.89553000000000005</v>
+      </c>
+      <c r="N122">
+        <v>2.5500000000000002E-3</v>
+      </c>
+      <c r="AW122" s="18">
         <v>0.92306999999999995</v>
       </c>
-      <c r="AX122">
+      <c r="AX122" s="18">
         <v>-7.6899999999999998E-3</v>
       </c>
     </row>
-    <row r="123" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW123">
+    <row r="123" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M123">
+        <v>0.91827400000000003</v>
+      </c>
+      <c r="N123">
+        <v>4.6979999999999999E-3</v>
+      </c>
+      <c r="AW123" s="18">
         <v>0.93571000000000004</v>
       </c>
-      <c r="AX123">
+      <c r="AX123" s="18">
         <v>-6.5399999999999998E-3</v>
       </c>
     </row>
-    <row r="124" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW124">
+    <row r="124" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M124">
+        <v>0.95184000000000002</v>
+      </c>
+      <c r="N124">
+        <v>9.0799999999999995E-3</v>
+      </c>
+      <c r="AW124" s="18">
         <v>0.94833000000000001</v>
       </c>
-      <c r="AX124">
+      <c r="AX124" s="18">
         <v>-5.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="125" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW125">
+    <row r="125" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M125">
+        <v>0.98662000000000005</v>
+      </c>
+      <c r="N125">
+        <v>1.4109999999999999E-2</v>
+      </c>
+      <c r="AW125" s="18">
         <v>0.96091000000000004</v>
       </c>
-      <c r="AX125">
+      <c r="AX125" s="18">
         <v>-4.28E-3</v>
       </c>
     </row>
-    <row r="126" spans="49:50" x14ac:dyDescent="0.25">
-      <c r="AW126">
+    <row r="126" spans="13:50" x14ac:dyDescent="0.25">
+      <c r="M126">
+        <v>0.99839</v>
+      </c>
+      <c r="N126">
+        <v>1.5949999999999999E-2</v>
+      </c>
+      <c r="AW126" s="18">
         <v>1</v>
       </c>
-      <c r="AX126">
+      <c r="AX126" s="18">
         <v>6.9999999999999999E-4</v>
       </c>
     </row>

</xml_diff>